<commit_message>
4th iteration - Complete
This detection algorithm is now very highly refined. It can detect over 90% of SLEs onset and offset with high accuracy.

However, some minor issues with labelling whether SLEs are light-triggered.

Future iterations will set the threshold for detecting artifacts based on a multiple of sigma.

Should also justify the spike detection thresholds
</commit_message>
<xml_diff>
--- a/13226009.xlsx
+++ b/13226009.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Seizure-Detection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E8A23259-181D-488C-BD18-3EB976FAEFC5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11445" windowHeight="7515"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11445" windowHeight="7515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental Protocol #1" sheetId="1" r:id="rId1"/>
     <sheet name="Interictal Events" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="25">
   <si>
     <t>Stim time (s)</t>
   </si>
@@ -81,13 +82,28 @@
   </si>
   <si>
     <t>Sub-seizure event?</t>
+  </si>
+  <si>
+    <t>Humans</t>
+  </si>
+  <si>
+    <t>Onset</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Algo - 4*sigma</t>
+  </si>
+  <si>
+    <t>Algo - 6*sigma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +132,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +171,16 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -160,17 +208,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -507,11 +563,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +582,7 @@
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,8 +610,19 @@
       <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>692.08280000000002</v>
       </c>
@@ -586,8 +653,26 @@
       <c r="I2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>843.80380000000002</v>
       </c>
@@ -618,8 +703,26 @@
       <c r="I3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>692.10890000000006</v>
+      </c>
+      <c r="L3">
+        <v>738.84760000000006</v>
+      </c>
+      <c r="M3" s="4">
+        <v>386.59019999999998</v>
+      </c>
+      <c r="N3" s="4">
+        <v>761.15170000000001</v>
+      </c>
+      <c r="O3" s="5">
+        <v>692.17110000000002</v>
+      </c>
+      <c r="P3" s="6">
+        <v>747.87400000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>995.52139999999997</v>
       </c>
@@ -650,8 +753,26 @@
       <c r="I4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>843.83080000000007</v>
+      </c>
+      <c r="L4">
+        <v>915.50010000000009</v>
+      </c>
+      <c r="M4" s="5">
+        <v>843.83109999999999</v>
+      </c>
+      <c r="N4" s="5">
+        <v>914.96</v>
+      </c>
+      <c r="O4" s="5">
+        <v>843.83109999999999</v>
+      </c>
+      <c r="P4" s="5">
+        <v>914.96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1118.1713999999999</v>
       </c>
@@ -682,8 +803,26 @@
       <c r="I5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>995.54829999999993</v>
+      </c>
+      <c r="L5">
+        <v>1040.809</v>
+      </c>
+      <c r="M5" s="5">
+        <v>995.54960000000005</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1056.5477000000001</v>
+      </c>
+      <c r="O5" s="5">
+        <v>995.54960000000005</v>
+      </c>
+      <c r="P5" s="4">
+        <v>1056.5477000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1317.1717000000001</v>
       </c>
@@ -714,8 +853,26 @@
       <c r="I6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>1118.2051999999999</v>
+      </c>
+      <c r="L6">
+        <v>1181.2822999999999</v>
+      </c>
+      <c r="M6" s="5">
+        <v>1118.2012</v>
+      </c>
+      <c r="N6" s="5">
+        <v>1180.664</v>
+      </c>
+      <c r="O6" s="5">
+        <v>1118.2012</v>
+      </c>
+      <c r="P6" s="5">
+        <v>1180.664</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1480.1074000000001</v>
       </c>
@@ -746,9 +903,27 @@
       <c r="I7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="K7">
+        <v>1317.1990000000001</v>
+      </c>
+      <c r="L7">
+        <v>1376.3197</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1317.2787000000001</v>
+      </c>
+      <c r="N7" s="4">
+        <v>1397.4315999999999</v>
+      </c>
+      <c r="O7" s="5">
+        <v>1317.2787000000001</v>
+      </c>
+      <c r="P7" s="4">
+        <v>1397.4315999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>1581.9540999999999</v>
       </c>
       <c r="B8">
@@ -778,8 +953,26 @@
       <c r="I8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>1480.1411000000001</v>
+      </c>
+      <c r="L8">
+        <v>1550.8947000000001</v>
+      </c>
+      <c r="M8" s="5">
+        <v>1480.1383000000001</v>
+      </c>
+      <c r="N8" s="5">
+        <v>1550.5255999999999</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1480.1383000000001</v>
+      </c>
+      <c r="P8" s="5">
+        <v>1550.5255999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1683.7995000000001</v>
       </c>
@@ -810,8 +1003,26 @@
       <c r="I9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>1581.9865</v>
+      </c>
+      <c r="L9">
+        <v>1635.1211000000001</v>
+      </c>
+      <c r="M9" s="5">
+        <v>1581.9871000000001</v>
+      </c>
+      <c r="N9" s="5">
+        <v>1633.5979</v>
+      </c>
+      <c r="O9" s="4">
+        <v>1592.4413</v>
+      </c>
+      <c r="P9" s="5">
+        <v>1633.5979</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1887.4851000000001</v>
       </c>
@@ -842,8 +1053,26 @@
       <c r="I10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>1683.8302000000001</v>
+      </c>
+      <c r="L10">
+        <v>1771.3882000000001</v>
+      </c>
+      <c r="M10" s="5">
+        <v>1683.8312000000001</v>
+      </c>
+      <c r="N10" s="5">
+        <v>1770.6265000000001</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1683.8312000000001</v>
+      </c>
+      <c r="P10" s="5">
+        <v>1770.6265000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2091.1595000000002</v>
       </c>
@@ -874,8 +1103,26 @@
       <c r="I11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>1887.5141000000001</v>
+      </c>
+      <c r="L11">
+        <v>1982.2073</v>
+      </c>
+      <c r="M11" s="5">
+        <v>1887.6111000000001</v>
+      </c>
+      <c r="N11" s="4">
+        <v>1989.3570999999999</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1887.6111000000001</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1989.3570999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2294.8366999999998</v>
       </c>
@@ -906,8 +1153,26 @@
       <c r="I12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>2091.1911</v>
+      </c>
+      <c r="L12">
+        <v>2186.4101000000001</v>
+      </c>
+      <c r="M12" s="5">
+        <v>2091.2858999999999</v>
+      </c>
+      <c r="N12" s="4">
+        <v>2231.433</v>
+      </c>
+      <c r="O12" s="5">
+        <v>2091.2858999999999</v>
+      </c>
+      <c r="P12" s="4">
+        <v>2231.433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2498.5001000000002</v>
       </c>
@@ -938,8 +1203,26 @@
       <c r="I13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>2294.8737999999998</v>
+      </c>
+      <c r="L13">
+        <v>2363.7217999999998</v>
+      </c>
+      <c r="M13" s="5">
+        <v>2294.8715000000002</v>
+      </c>
+      <c r="N13" s="5">
+        <v>2363.5369999999998</v>
+      </c>
+      <c r="O13" s="5">
+        <v>2294.8715000000002</v>
+      </c>
+      <c r="P13" s="5">
+        <v>2363.5369999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2702.165</v>
       </c>
@@ -970,8 +1253,26 @@
       <c r="I14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>2498.5335</v>
+      </c>
+      <c r="L14">
+        <v>2610.7525999999998</v>
+      </c>
+      <c r="M14" s="5">
+        <v>2498.6421</v>
+      </c>
+      <c r="N14" s="5">
+        <v>2610.6125999999999</v>
+      </c>
+      <c r="O14" s="5">
+        <v>2498.6421</v>
+      </c>
+      <c r="P14" s="5">
+        <v>2610.6125999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2905.8276000000001</v>
       </c>
@@ -1002,8 +1303,26 @@
       <c r="I15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>2702.2017999999998</v>
+      </c>
+      <c r="L15">
+        <v>2795.4930999999997</v>
+      </c>
+      <c r="M15" s="5">
+        <v>2702.2001</v>
+      </c>
+      <c r="N15" s="4">
+        <v>2838.835</v>
+      </c>
+      <c r="O15" s="5">
+        <v>2702.2001</v>
+      </c>
+      <c r="P15" s="4">
+        <v>2838.835</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3109.4859000000001</v>
       </c>
@@ -1034,8 +1353,26 @@
       <c r="I16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>2905.8652000000002</v>
+      </c>
+      <c r="L16">
+        <v>2997.6413000000002</v>
+      </c>
+      <c r="M16" s="5">
+        <v>2905.8638999999998</v>
+      </c>
+      <c r="N16" s="5">
+        <v>2997.3642</v>
+      </c>
+      <c r="O16" s="5">
+        <v>2905.8638999999998</v>
+      </c>
+      <c r="P16" s="5">
+        <v>2997.3642</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3314.0459999999998</v>
       </c>
@@ -1066,8 +1403,26 @@
       <c r="I17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>3109.5308</v>
+      </c>
+      <c r="L17">
+        <v>3199.7968000000001</v>
+      </c>
+      <c r="M17" s="5">
+        <v>3007.6918999999998</v>
+      </c>
+      <c r="N17" s="4">
+        <v>3037.7995000000001</v>
+      </c>
+      <c r="O17" s="5">
+        <v>3007.6918999999998</v>
+      </c>
+      <c r="P17" s="4">
+        <v>3037.7995000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3517.7026000000001</v>
       </c>
@@ -1097,6 +1452,44 @@
       </c>
       <c r="I18" t="s">
         <v>11</v>
+      </c>
+      <c r="K18">
+        <v>3314.0886999999998</v>
+      </c>
+      <c r="L18">
+        <v>3384.7324999999996</v>
+      </c>
+      <c r="M18" s="5">
+        <v>3314.1644000000001</v>
+      </c>
+      <c r="N18" s="5">
+        <v>3384.4395</v>
+      </c>
+      <c r="O18" s="5">
+        <v>3314.1644000000001</v>
+      </c>
+      <c r="P18" s="5">
+        <v>3384.4395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>3517.7399</v>
+      </c>
+      <c r="L19">
+        <v>3605.1507999999999</v>
+      </c>
+      <c r="M19" s="5">
+        <v>3517.8436999999999</v>
+      </c>
+      <c r="N19" s="5">
+        <v>3604.5632000000001</v>
+      </c>
+      <c r="O19" s="5">
+        <v>3517.8436999999999</v>
+      </c>
+      <c r="P19" s="5">
+        <v>3604.5632000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1106,7 +1499,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1790,7 +2183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Testing new artifact thresholds
I used threshold for artifacts to be avg + sigma*100

I should also use the threshold for epileptiform spikes to be avg + sigma*6

The algorithm is running very well and detecting points as described.

Artifacts are not being detect correctly

need to confirm false positives are not just real seizures missed by humans
</commit_message>
<xml_diff>
--- a/13226009.xlsx
+++ b/13226009.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E8A23259-181D-488C-BD18-3EB976FAEFC5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA4C2909-2AF1-4FE4-B288-CB92D32FE76E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11445" windowHeight="7515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,42 @@
     <sheet name="Interictal Events" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Michael Chang</author>
+  </authors>
+  <commentList>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{2AF437C6-DDE5-41F4-B342-01EF59B14A29}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Chang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the multiple we decided to use as the threshold to detect spikes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -103,7 +137,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +187,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -563,11 +610,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +665,7 @@
         <v>23</v>
       </c>
       <c r="N1" s="7"/>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1495,6 +1542,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
accurate detection - checkpoint
I am able to accurately detect the onset/offset of SLE and IISs using different techniques
</commit_message>
<xml_diff>
--- a/13226009.xlsx
+++ b/13226009.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA4C2909-2AF1-4FE4-B288-CB92D32FE76E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E6CA2CF5-DC76-4E7E-B507-085EAD584E32}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11445" windowHeight="7515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Interictal Events" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="26">
   <si>
     <t>Stim time (s)</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Algo - 6*sigma</t>
+  </si>
+  <si>
+    <t>V3.0</t>
   </si>
 </sst>
 </file>
@@ -611,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +632,7 @@
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,8 +671,11 @@
       <c r="O1" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>692.08280000000002</v>
       </c>
@@ -719,7 +725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>843.80380000000002</v>
       </c>
@@ -768,8 +774,14 @@
       <c r="P3" s="6">
         <v>747.87400000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>692.12159999999994</v>
+      </c>
+      <c r="R3">
+        <v>748.09059999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>995.52139999999997</v>
       </c>
@@ -818,8 +830,14 @@
       <c r="P4" s="5">
         <v>914.96</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>843.83699999999999</v>
+      </c>
+      <c r="R4">
+        <v>915.29319999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1118.1713999999999</v>
       </c>
@@ -868,8 +886,14 @@
       <c r="P5" s="4">
         <v>1056.5477000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>995.55960000000005</v>
+      </c>
+      <c r="R5">
+        <v>1056.7751000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1317.1717000000001</v>
       </c>
@@ -918,8 +942,14 @@
       <c r="P6" s="5">
         <v>1180.664</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>1118.2159999999999</v>
+      </c>
+      <c r="R6">
+        <v>1181.028</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1480.1074000000001</v>
       </c>
@@ -968,8 +998,14 @@
       <c r="P7" s="4">
         <v>1397.4315999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>1317.2126000000001</v>
+      </c>
+      <c r="R7">
+        <v>1398.0115000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1581.9540999999999</v>
       </c>
@@ -1018,8 +1054,14 @@
       <c r="P8" s="5">
         <v>1550.5255999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>1480.1541</v>
+      </c>
+      <c r="R8">
+        <v>1550.7545</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1683.7995000000001</v>
       </c>
@@ -1068,8 +1110,14 @@
       <c r="P9" s="5">
         <v>1633.5979</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>1592.4323999999999</v>
+      </c>
+      <c r="R9">
+        <v>1634.165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1887.4851000000001</v>
       </c>
@@ -1118,8 +1166,14 @@
       <c r="P10" s="5">
         <v>1770.6265000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>1683.8448000000001</v>
+      </c>
+      <c r="R10">
+        <v>1771.1962000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2091.1595000000002</v>
       </c>
@@ -1168,8 +1222,14 @@
       <c r="P11" s="4">
         <v>1989.3570999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>1887.5305000000001</v>
+      </c>
+      <c r="R11">
+        <v>1989.6387999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2294.8366999999998</v>
       </c>
@@ -1218,8 +1278,14 @@
       <c r="P12" s="4">
         <v>2231.433</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>2091.2091999999998</v>
+      </c>
+      <c r="R12">
+        <v>2232.4328999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2498.5001000000002</v>
       </c>
@@ -1268,8 +1334,14 @@
       <c r="P13" s="5">
         <v>2363.5369999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>2294.8859000000002</v>
+      </c>
+      <c r="R13">
+        <v>2363.7626</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2702.165</v>
       </c>
@@ -1318,8 +1390,14 @@
       <c r="P14" s="5">
         <v>2610.6125999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>2498.511</v>
+      </c>
+      <c r="R14">
+        <v>2610.8400999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2905.8276000000001</v>
       </c>
@@ -1368,8 +1446,14 @@
       <c r="P15" s="4">
         <v>2838.835</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>2702.1761000000001</v>
+      </c>
+      <c r="R15">
+        <v>2839.0929999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3109.4859000000001</v>
       </c>
@@ -1418,8 +1502,14 @@
       <c r="P16" s="5">
         <v>2997.3642</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>2905.8809999999999</v>
+      </c>
+      <c r="R16">
+        <v>2997.6118999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3314.0459999999998</v>
       </c>
@@ -1468,8 +1558,14 @@
       <c r="P17" s="4">
         <v>3037.7995000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>3109.4974000000002</v>
+      </c>
+      <c r="R17">
+        <v>3199.6738999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3517.7026000000001</v>
       </c>
@@ -1518,8 +1614,14 @@
       <c r="P18" s="5">
         <v>3384.4395</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>3314.0958999999998</v>
+      </c>
+      <c r="R18">
+        <v>3384.6698999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K19">
         <v>3517.7399</v>
       </c>
@@ -1537,6 +1639,12 @@
       </c>
       <c r="P19" s="5">
         <v>3604.5632000000001</v>
+      </c>
+      <c r="Q19">
+        <v>3517.7127999999998</v>
+      </c>
+      <c r="R19">
+        <v>3604.9576999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>